<commit_message>
Bug fixes en QoL things
</commit_message>
<xml_diff>
--- a/files/Admin/Bestand1.xlsx
+++ b/files/Admin/Bestand1.xlsx
@@ -1,3 +1,59 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Bestand2Sheet" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+</workbook>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  </cellStyles>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+</styleSheet>
+</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -258,4 +314,278 @@
     </a:ext>
   </a:extLst>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AB12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AB12" sqref="AB12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="15.7109375"/>
+    <col customWidth="1" max="2" min="2" width="33.85546875"/>
+    <col customWidth="1" max="3" min="3" width="29.85546875"/>
+    <col customWidth="1" max="28" min="28" width="24.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Dit is bestand 1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Dit is bestand 1 column 2</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Data bestand 1</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>Dit is bestand 1 column 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Test5423</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>dwadwa</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Test9432</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>dwadwa</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Test44242</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>dada</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Test74674</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 5</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>data bestaadand 1</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Test9424242</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 6</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dada</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Test342356</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 7</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>dwadwa</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Test12345</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 8</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Test1234479</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 9</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>wasdwa</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Test1237777</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 10</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>dwadwa</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Test4444</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 11</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>sdwa</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>Bestand 1 column 12</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test commit for creating a new release
</commit_message>
<xml_diff>
--- a/files/Admin/Bestand1.xlsx
+++ b/files/Admin/Bestand1.xlsx
@@ -338,7 +338,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Dit is bestand 1</t>
+          <t>&lt;br&gt; Dit is bestand 1 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -355,7 +355,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Test5</t>
+          <t>&lt;br&gt; Test5 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -367,7 +367,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Test9</t>
+          <t>&lt;br&gt; Test9 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -379,7 +379,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Test4</t>
+          <t>&lt;br&gt; Test4 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -391,7 +391,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Test7</t>
+          <t>&lt;br&gt; Test7 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -403,7 +403,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Test9</t>
+          <t>&lt;br&gt; Test9 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -415,7 +415,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Test3</t>
+          <t>&lt;br&gt; Test3 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -427,7 +427,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Test12345</t>
+          <t>&lt;br&gt; Test12345 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -439,7 +439,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Test1234479</t>
+          <t>&lt;br&gt; Test1234479 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -451,7 +451,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Test1237777</t>
+          <t>&lt;br&gt; Test1237777 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -463,7 +463,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Test4444</t>
+          <t>&lt;br&gt; Test4444 &lt;br /&gt;</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">

</xml_diff>